<commit_message>
1.add cast for litjson
</commit_message>
<xml_diff>
--- a/Assets/Resource/Table/Buff.xlsx
+++ b/Assets/Resource/Table/Buff.xlsx
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="118">
   <si>
     <t>buffid</t>
   </si>
@@ -168,184 +168,277 @@
     <t>[-20]</t>
   </si>
   <si>
+    <t>Effect/001</t>
+  </si>
+  <si>
     <t>["attack*1.6"]</t>
   </si>
   <si>
     <t>[-21]</t>
   </si>
   <si>
+    <t>Effect/002</t>
+  </si>
+  <si>
     <t>["attack*1.7"]</t>
   </si>
   <si>
     <t>[-22]</t>
   </si>
   <si>
+    <t>Effect/003</t>
+  </si>
+  <si>
     <t>["attack*1.8"]</t>
   </si>
   <si>
     <t>[-23]</t>
   </si>
   <si>
+    <t>Effect/004</t>
+  </si>
+  <si>
     <t>["attack*1.9"]</t>
   </si>
   <si>
     <t>[-24]</t>
   </si>
   <si>
+    <t>Effect/005</t>
+  </si>
+  <si>
     <t>["attack*1.10"]</t>
   </si>
   <si>
     <t>[-25]</t>
   </si>
   <si>
+    <t>Effect/006</t>
+  </si>
+  <si>
     <t>["attack*1.11"]</t>
   </si>
   <si>
     <t>[-26]</t>
   </si>
   <si>
+    <t>Effect/007</t>
+  </si>
+  <si>
     <t>["attack*1.12"]</t>
   </si>
   <si>
     <t>[-27]</t>
   </si>
   <si>
+    <t>Effect/008</t>
+  </si>
+  <si>
     <t>["attack*1.13"]</t>
   </si>
   <si>
     <t>[-28]</t>
   </si>
   <si>
+    <t>Effect/009</t>
+  </si>
+  <si>
     <t>["attack*1.14"]</t>
   </si>
   <si>
     <t>[-29]</t>
   </si>
   <si>
+    <t>Effect/010</t>
+  </si>
+  <si>
     <t>["attack*1.15"]</t>
   </si>
   <si>
     <t>[-30]</t>
   </si>
   <si>
+    <t>Effect/011</t>
+  </si>
+  <si>
     <t>["attack*1.16"]</t>
   </si>
   <si>
     <t>[-31]</t>
   </si>
   <si>
+    <t>Effect/012</t>
+  </si>
+  <si>
     <t>["attack*1.17"]</t>
   </si>
   <si>
     <t>[-32]</t>
   </si>
   <si>
+    <t>Effect/013</t>
+  </si>
+  <si>
     <t>["attack*1.18"]</t>
   </si>
   <si>
     <t>[-33]</t>
   </si>
   <si>
+    <t>Effect/014</t>
+  </si>
+  <si>
     <t>["attack*1.19"]</t>
   </si>
   <si>
     <t>[-34]</t>
   </si>
   <si>
+    <t>Effect/015</t>
+  </si>
+  <si>
     <t>["attack*1.20"]</t>
   </si>
   <si>
     <t>[-35]</t>
   </si>
   <si>
+    <t>Effect/016</t>
+  </si>
+  <si>
     <t>["attack*1.21"]</t>
   </si>
   <si>
     <t>[-36]</t>
   </si>
   <si>
+    <t>Effect/017</t>
+  </si>
+  <si>
     <t>["attack*1.22"]</t>
   </si>
   <si>
     <t>[-37]</t>
   </si>
   <si>
+    <t>Effect/018</t>
+  </si>
+  <si>
     <t>["attack*1.23"]</t>
   </si>
   <si>
     <t>[-38]</t>
   </si>
   <si>
+    <t>Effect/019</t>
+  </si>
+  <si>
     <t>["attack*1.24"]</t>
   </si>
   <si>
     <t>[-39]</t>
   </si>
   <si>
+    <t>Effect/020</t>
+  </si>
+  <si>
     <t>["attack*1.25"]</t>
   </si>
   <si>
     <t>[-40]</t>
   </si>
   <si>
+    <t>Effect/021</t>
+  </si>
+  <si>
     <t>["attack*1.26"]</t>
   </si>
   <si>
     <t>[-41]</t>
   </si>
   <si>
+    <t>Effect/022</t>
+  </si>
+  <si>
     <t>["attack*1.27"]</t>
   </si>
   <si>
     <t>[-42]</t>
   </si>
   <si>
+    <t>Effect/023</t>
+  </si>
+  <si>
     <t>["attack*1.28"]</t>
   </si>
   <si>
     <t>[-43]</t>
   </si>
   <si>
+    <t>Effect/024</t>
+  </si>
+  <si>
     <t>["attack*1.29"]</t>
   </si>
   <si>
     <t>[-44]</t>
   </si>
   <si>
+    <t>Effect/025</t>
+  </si>
+  <si>
     <t>["attack*1.30"]</t>
   </si>
   <si>
     <t>[-45]</t>
   </si>
   <si>
+    <t>Effect/026</t>
+  </si>
+  <si>
     <t>["attack*1.31"]</t>
   </si>
   <si>
     <t>[-46]</t>
   </si>
   <si>
+    <t>Effect/027</t>
+  </si>
+  <si>
     <t>["attack*1.32"]</t>
   </si>
   <si>
     <t>[-47]</t>
   </si>
   <si>
+    <t>Effect/028</t>
+  </si>
+  <si>
     <t>["attack*1.33"]</t>
   </si>
   <si>
     <t>[-48]</t>
   </si>
   <si>
+    <t>Effect/029</t>
+  </si>
+  <si>
     <t>["attack*1.34"]</t>
   </si>
   <si>
     <t>[-49]</t>
   </si>
   <si>
+    <t>Effect/030</t>
+  </si>
+  <si>
     <t>["attack*1.35"]</t>
   </si>
   <si>
     <t>[-50]</t>
+  </si>
+  <si>
+    <t>Effect/031</t>
   </si>
 </sst>
 </file>
@@ -366,12 +459,78 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -381,7 +540,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -411,27 +593,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -448,74 +609,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -530,19 +623,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,13 +791,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -572,145 +803,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -721,26 +814,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -759,17 +832,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -815,9 +882,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -829,10 +922,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -841,133 +934,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1300,7 +1393,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -1428,8 +1521,8 @@
       <c r="H4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="1">
-        <v>1111</v>
+      <c r="I4" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1452,13 +1545,13 @@
         <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1112</v>
+        <v>29</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1481,13 +1574,13 @@
         <v>24</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1113</v>
+        <v>32</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1510,13 +1603,13 @@
         <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1114</v>
+        <v>35</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1539,13 +1632,13 @@
         <v>24</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="1">
-        <v>1115</v>
+        <v>38</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1568,13 +1661,13 @@
         <v>24</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="1">
-        <v>1116</v>
+        <v>41</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1597,13 +1690,13 @@
         <v>24</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="1">
-        <v>1117</v>
+        <v>44</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1626,13 +1719,13 @@
         <v>24</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="1">
-        <v>1118</v>
+        <v>47</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1655,13 +1748,13 @@
         <v>24</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="1">
-        <v>1119</v>
+        <v>50</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1684,13 +1777,13 @@
         <v>24</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13" s="1">
-        <v>1120</v>
+        <v>53</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1713,13 +1806,13 @@
         <v>24</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I14" s="1">
-        <v>1121</v>
+        <v>56</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1742,13 +1835,13 @@
         <v>24</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I15" s="1">
-        <v>1122</v>
+        <v>59</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1771,13 +1864,13 @@
         <v>24</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="1">
-        <v>1123</v>
+        <v>62</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1800,13 +1893,13 @@
         <v>24</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="1">
-        <v>1124</v>
+        <v>65</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1829,13 +1922,13 @@
         <v>24</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I18" s="1">
-        <v>1125</v>
+        <v>68</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1858,13 +1951,13 @@
         <v>24</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" s="1">
-        <v>1126</v>
+        <v>71</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1887,13 +1980,13 @@
         <v>24</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I20" s="1">
-        <v>1127</v>
+        <v>74</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1916,13 +2009,13 @@
         <v>24</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I21" s="1">
-        <v>1128</v>
+        <v>77</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1945,13 +2038,13 @@
         <v>24</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I22" s="1">
-        <v>1129</v>
+        <v>80</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1974,13 +2067,13 @@
         <v>24</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I23" s="1">
-        <v>1130</v>
+        <v>83</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -2003,13 +2096,13 @@
         <v>24</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I24" s="1">
-        <v>1131</v>
+        <v>86</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2032,13 +2125,13 @@
         <v>24</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I25" s="1">
-        <v>1132</v>
+        <v>89</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2061,13 +2154,13 @@
         <v>24</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I26" s="1">
-        <v>1133</v>
+        <v>92</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -2090,13 +2183,13 @@
         <v>24</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I27" s="1">
-        <v>1134</v>
+        <v>95</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2119,13 +2212,13 @@
         <v>24</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I28" s="1">
-        <v>1135</v>
+        <v>98</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2148,13 +2241,13 @@
         <v>24</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I29" s="1">
-        <v>1136</v>
+        <v>101</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -2177,13 +2270,13 @@
         <v>24</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I30" s="1">
-        <v>1137</v>
+        <v>104</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2206,13 +2299,13 @@
         <v>24</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I31" s="1">
-        <v>1138</v>
+        <v>107</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2235,13 +2328,13 @@
         <v>24</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I32" s="1">
-        <v>1139</v>
+        <v>110</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -2264,13 +2357,13 @@
         <v>24</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I33" s="1">
-        <v>1140</v>
+        <v>113</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -2293,13 +2386,13 @@
         <v>24</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I34" s="1">
-        <v>1141</v>
+        <v>116</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>